<commit_message>
Liệt kê Actors của hệ thống.
</commit_message>
<xml_diff>
--- a/doc/design/GW_Design.xlsx
+++ b/doc/design/GW_Design.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="15480" windowHeight="8130" tabRatio="705"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="15480" windowHeight="8130" tabRatio="705" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Record of change" sheetId="1" r:id="rId1"/>
-    <sheet name="Architecture design" sheetId="22" r:id="rId2"/>
-    <sheet name="Screen design" sheetId="21" r:id="rId3"/>
+    <sheet name="Screen design" sheetId="21" r:id="rId2"/>
+    <sheet name="Architecture design" sheetId="22" r:id="rId3"/>
     <sheet name="Domain design" sheetId="23" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -121,6 +121,46 @@
   <si>
     <t>Design</t>
   </si>
+  <si>
+    <t>Screen design</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Trên cơ sở tài liệu trong thư mục "Requirement", tài liệu này phát thảo màn hình cho các nhóm người dùng của hệ thống bao gồm:</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>Người quản trị hệ thống của nhà cung cấp dịch vụ (Supplier)</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>Người quản lý khách hàng của nhà cung cấp dịch vụ</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>Nhân viên chăm sóc khách hàng của nhà cung cấp dịch vụ</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>Người quản trị dịch vụ của bên sử dụng dịch vụ (Consumer)</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>Nhân viên sử dụng dịch vụ của bên sử dụng dịch vụ</t>
+  </si>
 </sst>
 </file>
 
@@ -131,7 +171,7 @@
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="dd\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="43">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -393,6 +433,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
     </font>
   </fonts>
   <fills count="26">
@@ -1056,7 +1102,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="23" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1345,6 +1391,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1790,7 +1837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1995,8 +2042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU35"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AG3" sqref="AG3:AJ3"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15"/>
@@ -2092,7 +2139,9 @@
       <c r="B3" s="92"/>
       <c r="C3" s="92"/>
       <c r="D3" s="92"/>
-      <c r="E3" s="95"/>
+      <c r="E3" s="95" t="s">
+        <v>21</v>
+      </c>
       <c r="F3" s="96"/>
       <c r="G3" s="96"/>
       <c r="H3" s="97"/>
@@ -2102,7 +2151,9 @@
       <c r="J3" s="92"/>
       <c r="K3" s="92"/>
       <c r="L3" s="101"/>
-      <c r="M3" s="103"/>
+      <c r="M3" s="103" t="s">
+        <v>20</v>
+      </c>
       <c r="N3" s="96"/>
       <c r="O3" s="96"/>
       <c r="P3" s="96"/>
@@ -2255,7 +2306,9 @@
     </row>
     <row r="7" spans="1:47" ht="15.75">
       <c r="A7" s="40"/>
-      <c r="B7" s="42"/>
+      <c r="B7" s="42" t="s">
+        <v>22</v>
+      </c>
       <c r="C7" s="42"/>
       <c r="D7" s="42"/>
       <c r="E7" s="42"/>
@@ -2294,8 +2347,12 @@
     <row r="8" spans="1:47" ht="15.75">
       <c r="A8" s="40"/>
       <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
+      <c r="C8" s="112" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>24</v>
+      </c>
       <c r="E8" s="41"/>
       <c r="F8" s="53"/>
       <c r="G8" s="53"/>
@@ -2332,8 +2389,12 @@
     <row r="9" spans="1:47" ht="15.75">
       <c r="A9" s="40"/>
       <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
+      <c r="C9" s="112" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>26</v>
+      </c>
       <c r="E9" s="42"/>
       <c r="F9" s="42"/>
       <c r="G9" s="42"/>
@@ -2370,8 +2431,12 @@
     <row r="10" spans="1:47" ht="15.75">
       <c r="A10" s="46"/>
       <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
+      <c r="C10" s="112" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>28</v>
+      </c>
       <c r="E10" s="47"/>
       <c r="F10" s="42"/>
       <c r="G10" s="42"/>
@@ -2408,8 +2473,12 @@
     <row r="11" spans="1:47" ht="15.75">
       <c r="A11" s="49"/>
       <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
+      <c r="C11" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>30</v>
+      </c>
       <c r="E11" s="47"/>
       <c r="F11" s="42"/>
       <c r="G11" s="42"/>
@@ -2446,8 +2515,12 @@
     <row r="12" spans="1:47" ht="15.75">
       <c r="A12" s="49"/>
       <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
+      <c r="C12" s="112" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>32</v>
+      </c>
       <c r="E12" s="47"/>
       <c r="F12" s="42"/>
       <c r="G12" s="41"/>

</xml_diff>